<commit_message>
feat(EM): prep test build
</commit_message>
<xml_diff>
--- a/Emmersive/package/LangMod/emmersive_localizations.xlsx
+++ b/Emmersive/package/LangMod/emmersive_localizations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\Emmersive\package\LangMod\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF72B22-2950-4803-93E4-0B682C8912FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404FD38B-8550-4ABC-9821-DEEC8BB1D4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1350" yWindow="3570" windowWidth="33615" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="555" yWindow="705" windowWidth="33615" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="116">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -139,13 +139,256 @@
   </si>
   <si>
     <t>API Key</t>
+  </si>
+  <si>
+    <t>em_environment_data_date</t>
+  </si>
+  <si>
+    <t>em_environment_data_season</t>
+  </si>
+  <si>
+    <t>em_environment_data_weather</t>
+  </si>
+  <si>
+    <t>em_environment_data</t>
+  </si>
+  <si>
+    <t>em_zone_data_name</t>
+  </si>
+  <si>
+    <t>em_zone_data_allow_crime</t>
+  </si>
+  <si>
+    <t>em_zone_data_has_law</t>
+  </si>
+  <si>
+    <t>em_zone_data_is_town</t>
+  </si>
+  <si>
+    <t>em_zone_data_player_influence</t>
+  </si>
+  <si>
+    <t>em_zone_data</t>
+  </si>
+  <si>
+    <t>em_character_data_name</t>
+  </si>
+  <si>
+    <t>em_character_data_uid</t>
+  </si>
+  <si>
+    <t>em_character_data_title</t>
+  </si>
+  <si>
+    <t>em_character_data_level</t>
+  </si>
+  <si>
+    <t>em_character_data_hp</t>
+  </si>
+  <si>
+    <t>em_character_data_mana</t>
+  </si>
+  <si>
+    <t>em_character_data_stamina</t>
+  </si>
+  <si>
+    <t>em_character_data_class</t>
+  </si>
+  <si>
+    <t>em_character_data_race</t>
+  </si>
+  <si>
+    <t>em_character_data_age</t>
+  </si>
+  <si>
+    <t>em_character_data_gender</t>
+  </si>
+  <si>
+    <t>em_character_data_background</t>
+  </si>
+  <si>
+    <t>em_character_data_fame</t>
+  </si>
+  <si>
+    <t>em_player_data_name</t>
+  </si>
+  <si>
+    <t>em_player_data_uid</t>
+  </si>
+  <si>
+    <t>em_player_data_title</t>
+  </si>
+  <si>
+    <t>em_player_data_level</t>
+  </si>
+  <si>
+    <t>em_player_data_hp</t>
+  </si>
+  <si>
+    <t>em_player_data_mana</t>
+  </si>
+  <si>
+    <t>em_player_data_stamina</t>
+  </si>
+  <si>
+    <t>em_player_data_class</t>
+  </si>
+  <si>
+    <t>em_player_data_race</t>
+  </si>
+  <si>
+    <t>em_player_data_age</t>
+  </si>
+  <si>
+    <t>em_player_data_gender</t>
+  </si>
+  <si>
+    <t>em_player_data_background</t>
+  </si>
+  <si>
+    <t>em_player_data_fame</t>
+  </si>
+  <si>
+    <t>em_player_data</t>
+  </si>
+  <si>
+    <t>em_previous_action_log</t>
+  </si>
+  <si>
+    <t>em_character_data_hostility</t>
+  </si>
+  <si>
+    <t>em_character_data_affinity</t>
+  </si>
+  <si>
+    <t>em_character_data_in_party</t>
+  </si>
+  <si>
+    <t>em_character_data_faith</t>
+  </si>
+  <si>
+    <t>em_nearby_characters_characters</t>
+  </si>
+  <si>
+    <t>em_nearby_characters</t>
+  </si>
+  <si>
+    <t>em_scene_triggers</t>
+  </si>
+  <si>
+    <t>Environment Data</t>
+  </si>
+  <si>
+    <t>Weather</t>
+  </si>
+  <si>
+    <t>Season</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Zone Name</t>
+  </si>
+  <si>
+    <t>Allow Crime</t>
+  </si>
+  <si>
+    <t>Has Law</t>
+  </si>
+  <si>
+    <t>Is Civilized</t>
+  </si>
+  <si>
+    <t>Player Influence</t>
+  </si>
+  <si>
+    <t>Zone Data</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>uid</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Mana</t>
+  </si>
+  <si>
+    <t>Stamina</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Race</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Gender</t>
+  </si>
+  <si>
+    <t>Background</t>
+  </si>
+  <si>
+    <t>Fame</t>
+  </si>
+  <si>
+    <t>Player Data</t>
+  </si>
+  <si>
+    <t>Recent Actions Log</t>
+  </si>
+  <si>
+    <t>Hostility</t>
+  </si>
+  <si>
+    <t>Affinity With Player</t>
+  </si>
+  <si>
+    <t>In Player Party</t>
+  </si>
+  <si>
+    <t>Religion</t>
+  </si>
+  <si>
+    <t>Nearby Characters</t>
+  </si>
+  <si>
+    <t>Characters</t>
+  </si>
+  <si>
+    <t>Scene Triggers</t>
+  </si>
+  <si>
+    <t>em_ui_reload</t>
+  </si>
+  <si>
+    <t>em_ui_reload_prompts</t>
+  </si>
+  <si>
+    <t>Reload Prompts</t>
+  </si>
+  <si>
+    <t>Reload</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,37 +425,6 @@
       <name val="Cascadia Code"/>
       <family val="3"/>
     </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Cascadia Code"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <name val="Yu Gothic"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <name val="Cascadia Code"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Cascadia Code"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -234,7 +446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -242,22 +454,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -540,10 +737,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:D18"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="16.5"/>
@@ -585,13 +782,13 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="23.25">
-      <c r="A3" s="6"/>
+      <c r="A3" s="5"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
+      <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4" ht="23.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="5"/>
@@ -603,7 +800,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" ht="23.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="5"/>
@@ -615,7 +812,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" ht="23.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="5"/>
@@ -626,36 +823,36 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="25.5">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:4" ht="23.25">
+      <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="5"/>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="25.5">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:4" ht="23.25">
+      <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="5"/>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="25.5">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:4" ht="23.25">
+      <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="5"/>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -663,11 +860,11 @@
       </c>
     </row>
     <row r="10" spans="1:4" ht="23.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="5"/>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -675,23 +872,23 @@
       </c>
     </row>
     <row r="11" spans="1:4" ht="23.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="5"/>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="25.5">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:4" ht="23.25">
+      <c r="A12" s="5" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="5"/>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D12" s="5" t="s">
@@ -699,166 +896,718 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="23.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="5"/>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="3" customFormat="1" ht="23.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="5"/>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="23.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="5"/>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="23.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="5"/>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="46.5">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="5"/>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="23.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="5"/>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="23.25">
-      <c r="A19" s="6"/>
+      <c r="A19" s="5" t="s">
+        <v>112</v>
+      </c>
       <c r="B19" s="5"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="5"/>
+      <c r="C19" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="23.25">
-      <c r="A20" s="6"/>
+      <c r="A20" s="5" t="s">
+        <v>113</v>
+      </c>
       <c r="B20" s="5"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="5"/>
+      <c r="C20" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="23.25">
-      <c r="A21" s="6"/>
+      <c r="A21" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="B21" s="5"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="5"/>
+      <c r="C21" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="22" spans="1:4" ht="23.25">
-      <c r="A22" s="6"/>
+      <c r="A22" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="B22" s="5"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="5"/>
+      <c r="C22" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="23" spans="1:4" ht="23.25">
-      <c r="A23" s="6"/>
+      <c r="A23" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="B23" s="5"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="5"/>
+      <c r="C23" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="23.25">
-      <c r="A24" s="6"/>
+      <c r="A24" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="B24" s="5"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="5"/>
-    </row>
-    <row r="25" spans="1:4" s="3" customFormat="1" ht="23.25">
-      <c r="A25" s="6"/>
+      <c r="C24" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="23.25">
+      <c r="A25" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="B25" s="5"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="5"/>
+      <c r="C25" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="26" spans="1:4" ht="23.25">
-      <c r="A26" s="6"/>
+      <c r="A26" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="B26" s="5"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="5"/>
-    </row>
-    <row r="27" spans="1:4" ht="23.25">
-      <c r="A27" s="6"/>
+      <c r="C26" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="3" customFormat="1" ht="23.25">
+      <c r="A27" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="B27" s="5"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="5"/>
+      <c r="C27" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="28" spans="1:4" ht="23.25">
-      <c r="A28" s="6"/>
+      <c r="A28" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="B28" s="5"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="5"/>
+      <c r="C28" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="29" spans="1:4" ht="23.25">
-      <c r="A29" s="6"/>
+      <c r="A29" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="B29" s="5"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="5"/>
+      <c r="C29" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="30" spans="1:4" ht="23.25">
-      <c r="A30" s="6"/>
+      <c r="A30" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="B30" s="5"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="5"/>
+      <c r="C30" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="31" spans="1:4" ht="23.25">
-      <c r="A31" s="6"/>
+      <c r="A31" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="B31" s="5"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="5"/>
-    </row>
-    <row r="48" spans="1:4" s="2" customFormat="1">
-      <c r="A48" s="3"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="1"/>
-    </row>
-    <row r="49" spans="1:4" s="2" customFormat="1">
-      <c r="A49" s="3"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="1"/>
+      <c r="C31" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="23.25">
+      <c r="A32" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="23.25">
+      <c r="A33" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="23.25">
+      <c r="A34" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="23.25">
+      <c r="A35" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="23.25">
+      <c r="A36" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="23.25">
+      <c r="A37" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="23.25">
+      <c r="A38" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="23.25">
+      <c r="A39" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="23.25">
+      <c r="A40" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="23.25">
+      <c r="A41" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="23.25">
+      <c r="A42" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="23.25">
+      <c r="A43" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="23.25">
+      <c r="A44" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="23.25">
+      <c r="A45" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="23.25">
+      <c r="A46" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="23.25">
+      <c r="A47" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="23.25">
+      <c r="A48" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="23.25">
+      <c r="A49" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="2" customFormat="1" ht="23.25">
+      <c r="A50" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="2" customFormat="1" ht="23.25">
+      <c r="A51" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="23.25">
+      <c r="A52" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="23.25">
+      <c r="A53" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="23.25">
+      <c r="A54" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" s="5"/>
+      <c r="C54" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="23.25">
+      <c r="A55" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B55" s="5"/>
+      <c r="C55" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="23.25">
+      <c r="A56" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="23.25">
+      <c r="A57" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="23.25">
+      <c r="A58" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="23.25">
+      <c r="A59" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="23.25">
+      <c r="A60" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="23.25">
+      <c r="A61" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="D61" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="23.25">
+      <c r="A62" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="23.25">
+      <c r="A63" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63" s="5"/>
+      <c r="C63" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="23.25">
+      <c r="A64" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B64" s="5"/>
+      <c r="C64" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="23.25">
+      <c r="A65" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B65" s="5"/>
+      <c r="C65" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="23.25">
+      <c r="A66" s="5"/>
+      <c r="B66" s="5"/>
+      <c r="C66" s="5"/>
+      <c r="D66" s="5"/>
+    </row>
+    <row r="67" spans="1:4" ht="23.25">
+      <c r="A67" s="5"/>
+      <c r="B67" s="5"/>
+      <c r="C67" s="5"/>
+      <c r="D67" s="5"/>
+    </row>
+    <row r="68" spans="1:4" ht="23.25">
+      <c r="A68" s="5"/>
+      <c r="B68" s="5"/>
+      <c r="C68" s="5"/>
+      <c r="D68" s="5"/>
+    </row>
+    <row r="69" spans="1:4" ht="23.25">
+      <c r="A69" s="5"/>
+      <c r="B69" s="5"/>
+      <c r="C69" s="5"/>
+      <c r="D69" s="5"/>
+    </row>
+    <row r="70" spans="1:4" ht="23.25">
+      <c r="A70" s="5"/>
+      <c r="B70" s="5"/>
+      <c r="C70" s="5"/>
+      <c r="D70" s="5"/>
+    </row>
+    <row r="71" spans="1:4" ht="23.25">
+      <c r="A71" s="5"/>
+      <c r="B71" s="5"/>
+      <c r="C71" s="5"/>
+      <c r="D71" s="5"/>
+    </row>
+    <row r="72" spans="1:4" ht="23.25">
+      <c r="A72" s="5"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="5"/>
+      <c r="D72" s="5"/>
+    </row>
+    <row r="73" spans="1:4" ht="23.25">
+      <c r="A73" s="5"/>
+      <c r="B73" s="5"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+    </row>
+    <row r="74" spans="1:4" ht="23.25">
+      <c r="A74" s="5"/>
+      <c r="B74" s="5"/>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+    </row>
+    <row r="75" spans="1:4" ht="23.25">
+      <c r="A75" s="5"/>
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
+    </row>
+    <row r="76" spans="1:4" ht="23.25">
+      <c r="A76" s="5"/>
+      <c r="B76" s="5"/>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+    </row>
+    <row r="77" spans="1:4" ht="23.25">
+      <c r="A77" s="5"/>
+      <c r="B77" s="5"/>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+    </row>
+    <row r="78" spans="1:4" ht="23.25">
+      <c r="A78" s="5"/>
+      <c r="B78" s="5"/>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>